<commit_message>
fixes for generating excel (#30)
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/proposed.xlsx
+++ b/requirement/src/main/resources/templates/proposed.xlsx
@@ -497,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>